<commit_message>
Added data for original prediction model
</commit_message>
<xml_diff>
--- a/Results/results2.xlsx
+++ b/Results/results2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9660" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="KNN Err" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="18">
   <si>
     <t>userW</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>err</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
 </sst>
 </file>
@@ -692,7 +695,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>KNN MSE BaseLine</c:v>
+            <c:v>KNN Err BaseLine</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050">
@@ -833,7 +836,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>KNN MSE Weighted</c:v>
+            <c:v>KNN Err Weighted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050">
@@ -846,7 +849,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="triangle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
@@ -970,6 +973,145 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>KNN Err Weighted Original</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$E$62:$E$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$N$62:$N$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.58324607329842937</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56814310051107331</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55373831775700932</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55409356725146197</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.55129099790648983</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55259653794940078</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55736636245110827</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55834945196647323</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55676020408163263</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.55449936628643848</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5568110483364721</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55741775294847917</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.55679012345679013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.55644171779141105</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.55792682926829273</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -978,11 +1120,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276556264"/>
-        <c:axId val="276557832"/>
+        <c:axId val="7809040"/>
+        <c:axId val="7809432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276556264"/>
+        <c:axId val="7809040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,12 +1213,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276557832"/>
+        <c:crossAx val="7809432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276557832"/>
+        <c:axId val="7809432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1168,7 +1310,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276556264"/>
+        <c:crossAx val="7809040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1306,118 +1448,7 @@
           <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>PCA MSE BaseLine</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>results!$F$2:$F$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>200</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>results!$N$2:$N$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.53831294269156471</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.54035308953341743</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.53729456384323637</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.54134860050890588</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.54055766793409377</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.54240506329113924</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.54395951929158759</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.54395951929158759</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.54338188727042436</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.54395951929158759</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>PCA MSE Weighted</c:v>
+            <c:v>PCA Err BaseLine</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050">
@@ -1446,6 +1477,117 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>results!$F$2:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$N$2:$N$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.53831294269156471</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54035308953341743</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53729456384323637</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54134860050890588</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54055766793409377</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.54240506329113924</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.54395951929158759</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.54395951929158759</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.54338188727042436</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.54395951929158759</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>PCA Err Weighted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
               <c:f>results!$F$27:$F$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1518,6 +1660,113 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.54016445287792536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>PCA Err Weighted Original</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$F$52:$F$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$N$52:$N$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.56084996780424989</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55800756620428749</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55309734513274333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55852417302798985</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.55449936628643848</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5563291139240506</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55660974067046176</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55660974067046176</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55604813172894241</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.55597722960151807</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1532,11 +1781,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276559400"/>
-        <c:axId val="276559792"/>
+        <c:axId val="378871056"/>
+        <c:axId val="378871448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276559400"/>
+        <c:axId val="378871056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1630,16 +1879,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276559792"/>
+        <c:crossAx val="378871448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276559792"/>
+        <c:axId val="378871448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.55500000000000005"/>
-          <c:min val="0.51500000000000001"/>
+          <c:max val="0.59000000000000008"/>
+          <c:min val="0.51"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1734,7 +1983,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276559400"/>
+        <c:crossAx val="378871056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1884,11 +2133,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1991,15 +2240,15 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="triangle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2085,6 +2334,113 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>PCA MSE Weighted Original</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$F$52:$F$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$G$52:$G$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.64036188418999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.63967587265299997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63281929326999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63860196939000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63705571485800006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.63559681484599995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.63802119705399996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.63779668277099999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.636351915908</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.63600506526099998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2093,11 +2449,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276557048"/>
-        <c:axId val="276557440"/>
+        <c:axId val="378872232"/>
+        <c:axId val="378869488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276557048"/>
+        <c:axId val="378872232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2191,15 +2547,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276557440"/>
+        <c:crossAx val="378869488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276557440"/>
+        <c:axId val="378869488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.64000000000000012"/>
+          <c:max val="0.65500000000000014"/>
           <c:min val="0.60000000000000009"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2290,7 +2646,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276557048"/>
+        <c:crossAx val="378872232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2577,7 +2933,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="triangle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
@@ -2701,6 +3057,145 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>KNN MSE Weighted Original</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$E$62:$E$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$G$62:$G$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.64337080167399996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.647982783196</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.64409474417199997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64233188766399996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63864301690299996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.63645889307400005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.63807034950300001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.64224702654499999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.64171608867700003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.63705571485800006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.63750908140100004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.63686245617799997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.63204954909</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.63469454315600005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.63416869797700004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2709,11 +3204,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276555088"/>
-        <c:axId val="276561360"/>
+        <c:axId val="378873016"/>
+        <c:axId val="378869880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276555088"/>
+        <c:axId val="378873016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2802,12 +3297,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276561360"/>
+        <c:crossAx val="378869880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276561360"/>
+        <c:axId val="378869880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2899,7 +3394,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276555088"/>
+        <c:crossAx val="378873016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2977,7 +3472,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="53" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2988,7 +3483,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="53" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="93" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2999,7 +3494,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="53" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="93" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3010,7 +3505,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="93" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3021,7 +3516,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8655326" cy="6284429"/>
+    <xdr:ext cx="8664677" cy="6288548"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3048,7 +3543,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8655326" cy="6284429"/>
+    <xdr:ext cx="8664677" cy="6288548"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3075,7 +3570,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8655326" cy="6284429"/>
+    <xdr:ext cx="8664677" cy="6288548"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3102,7 +3597,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8655326" cy="6284429"/>
+    <xdr:ext cx="8674554" cy="6293304"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3388,10 +3883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3941,11 +4436,11 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" ref="M12:M33" si="2">SUM(H12:L12)</f>
+        <f t="shared" ref="M12:M26" si="2">SUM(H12:L12)</f>
         <v>955</v>
       </c>
       <c r="N12">
-        <f>(I12+J12*2+K12*3+L12*4)/M12</f>
+        <f t="shared" ref="N12:N26" si="3">(I12+J12*2+K12*3+L12*4)/M12</f>
         <v>0.52774869109947642</v>
       </c>
     </row>
@@ -3991,7 +4486,7 @@
         <v>1174</v>
       </c>
       <c r="N13">
-        <f>(I13+J13*2+K13*3+L13*4)/M13</f>
+        <f t="shared" si="3"/>
         <v>0.53833049403747868</v>
       </c>
     </row>
@@ -4037,7 +4532,7 @@
         <v>1285</v>
       </c>
       <c r="N14">
-        <f>(I14+J14*2+K14*3+L14*4)/M14</f>
+        <f t="shared" si="3"/>
         <v>0.54007782101167312</v>
       </c>
     </row>
@@ -4083,7 +4578,7 @@
         <v>1369</v>
       </c>
       <c r="N15">
-        <f>(I15+J15*2+K15*3+L15*4)/M15</f>
+        <f t="shared" si="3"/>
         <v>0.55003652300949601</v>
       </c>
     </row>
@@ -4129,7 +4624,7 @@
         <v>1434</v>
       </c>
       <c r="N16">
-        <f>(I16+J16*2+K16*3+L16*4)/M16</f>
+        <f t="shared" si="3"/>
         <v>0.54602510460251041</v>
       </c>
     </row>
@@ -4175,7 +4670,7 @@
         <v>1501</v>
       </c>
       <c r="N17">
-        <f>(I17+J17*2+K17*3+L17*4)/M17</f>
+        <f t="shared" si="3"/>
         <v>0.54297135243171224</v>
       </c>
     </row>
@@ -4221,7 +4716,7 @@
         <v>1535</v>
       </c>
       <c r="N18">
-        <f>(I18+J18*2+K18*3+L18*4)/M18</f>
+        <f t="shared" si="3"/>
         <v>0.53876221498371335</v>
       </c>
     </row>
@@ -4267,7 +4762,7 @@
         <v>1552</v>
       </c>
       <c r="N19">
-        <f>(I19+J19*2+K19*3+L19*4)/M19</f>
+        <f t="shared" si="3"/>
         <v>0.53737113402061853</v>
       </c>
     </row>
@@ -4313,7 +4808,7 @@
         <v>1569</v>
       </c>
       <c r="N20">
-        <f>(I20+J20*2+K20*3+L20*4)/M20</f>
+        <f t="shared" si="3"/>
         <v>0.53664754620777566</v>
       </c>
     </row>
@@ -4359,7 +4854,7 @@
         <v>1578</v>
       </c>
       <c r="N21">
-        <f>(I21+J21*2+K21*3+L21*4)/M21</f>
+        <f t="shared" si="3"/>
         <v>0.53612167300380231</v>
       </c>
     </row>
@@ -4405,7 +4900,7 @@
         <v>1593</v>
       </c>
       <c r="N22">
-        <f>(I22+J22*2+K22*3+L22*4)/M22</f>
+        <f t="shared" si="3"/>
         <v>0.53986189579409916</v>
       </c>
     </row>
@@ -4451,7 +4946,7 @@
         <v>1611</v>
       </c>
       <c r="N23">
-        <f>(I23+J23*2+K23*3+L23*4)/M23</f>
+        <f t="shared" si="3"/>
         <v>0.54127870887647422</v>
       </c>
     </row>
@@ -4497,7 +4992,7 @@
         <v>1620</v>
       </c>
       <c r="N24">
-        <f>(I24+J24*2+K24*3+L24*4)/M24</f>
+        <f t="shared" si="3"/>
         <v>0.5419753086419753</v>
       </c>
     </row>
@@ -4543,7 +5038,7 @@
         <v>1630</v>
       </c>
       <c r="N25">
-        <f>(I25+J25*2+K25*3+L25*4)/M25</f>
+        <f t="shared" si="3"/>
         <v>0.54539877300613493</v>
       </c>
     </row>
@@ -4589,7 +5084,7 @@
         <v>1640</v>
       </c>
       <c r="N26">
-        <f>(I26+J26*2+K26*3+L26*4)/M26</f>
+        <f t="shared" si="3"/>
         <v>0.54146341463414638</v>
       </c>
     </row>
@@ -4631,11 +5126,11 @@
         <v>0</v>
       </c>
       <c r="M27">
-        <f t="shared" ref="M27:M36" si="3">SUM(H27:L27)</f>
+        <f t="shared" ref="M27:M36" si="4">SUM(H27:L27)</f>
         <v>1553</v>
       </c>
       <c r="N27">
-        <f t="shared" ref="N27:N36" si="4">(I27+J27*2+K27*3+L27*4)/M27</f>
+        <f t="shared" ref="N27:N36" si="5">(I27+J27*2+K27*3+L27*4)/M27</f>
         <v>0.53573728267868637</v>
       </c>
     </row>
@@ -4677,11 +5172,11 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1586</v>
       </c>
       <c r="N28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.54098360655737709</v>
       </c>
     </row>
@@ -4723,11 +5218,11 @@
         <v>0</v>
       </c>
       <c r="M29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1582</v>
       </c>
       <c r="N29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.53729456384323637</v>
       </c>
     </row>
@@ -4769,11 +5264,11 @@
         <v>0</v>
       </c>
       <c r="M30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1572</v>
       </c>
       <c r="N30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.53689567430025442</v>
       </c>
     </row>
@@ -4815,11 +5310,11 @@
         <v>0</v>
       </c>
       <c r="M31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1578</v>
       </c>
       <c r="N31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.53612167300380231</v>
       </c>
     </row>
@@ -4861,11 +5356,11 @@
         <v>0</v>
       </c>
       <c r="M32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1580</v>
       </c>
       <c r="N32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.53860759493670884</v>
       </c>
     </row>
@@ -4907,11 +5402,11 @@
         <v>0</v>
       </c>
       <c r="M33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1581</v>
       </c>
       <c r="N33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.53889943074003799</v>
       </c>
     </row>
@@ -4953,11 +5448,11 @@
         <v>0</v>
       </c>
       <c r="M34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1581</v>
       </c>
       <c r="N34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.53953194180898167</v>
       </c>
     </row>
@@ -4999,11 +5494,11 @@
         <v>0</v>
       </c>
       <c r="M35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1579</v>
       </c>
       <c r="N35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.53958201393286886</v>
       </c>
     </row>
@@ -5045,11 +5540,11 @@
         <v>0</v>
       </c>
       <c r="M36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1581</v>
       </c>
       <c r="N36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.54016445287792536</v>
       </c>
     </row>
@@ -5091,11 +5586,11 @@
         <v>0</v>
       </c>
       <c r="M37">
-        <f t="shared" ref="M34:M51" si="5">SUM(H37:L37)</f>
+        <f t="shared" ref="M37:M51" si="6">SUM(H37:L37)</f>
         <v>955</v>
       </c>
       <c r="N37">
-        <f>(I37+J37*2+K37*3+L37*4)/M37</f>
+        <f t="shared" ref="N37:N51" si="7">(I37+J37*2+K37*3+L37*4)/M37</f>
         <v>0.51832460732984298</v>
       </c>
     </row>
@@ -5137,11 +5632,11 @@
         <v>0</v>
       </c>
       <c r="M38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1174</v>
       </c>
       <c r="N38">
-        <f>(I38+J38*2+K38*3+L38*4)/M38</f>
+        <f t="shared" si="7"/>
         <v>0.52725724020442932</v>
       </c>
     </row>
@@ -5183,11 +5678,11 @@
         <v>0</v>
       </c>
       <c r="M39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1285</v>
       </c>
       <c r="N39">
-        <f>(I39+J39*2+K39*3+L39*4)/M39</f>
+        <f t="shared" si="7"/>
         <v>0.53696498054474706</v>
       </c>
     </row>
@@ -5229,11 +5724,11 @@
         <v>0</v>
       </c>
       <c r="M40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1369</v>
       </c>
       <c r="N40">
-        <f>(I40+J40*2+K40*3+L40*4)/M40</f>
+        <f t="shared" si="7"/>
         <v>0.54200146092037982</v>
       </c>
     </row>
@@ -5275,11 +5770,11 @@
         <v>0</v>
       </c>
       <c r="M41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1434</v>
       </c>
       <c r="N41">
-        <f>(I41+J41*2+K41*3+L41*4)/M41</f>
+        <f t="shared" si="7"/>
         <v>0.54044630404463045</v>
       </c>
     </row>
@@ -5321,11 +5816,11 @@
         <v>0</v>
       </c>
       <c r="M42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1501</v>
       </c>
       <c r="N42">
-        <f>(I42+J42*2+K42*3+L42*4)/M42</f>
+        <f t="shared" si="7"/>
         <v>0.54097268487674888</v>
       </c>
     </row>
@@ -5367,11 +5862,11 @@
         <v>0</v>
       </c>
       <c r="M43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1535</v>
       </c>
       <c r="N43">
-        <f>(I43+J43*2+K43*3+L43*4)/M43</f>
+        <f t="shared" si="7"/>
         <v>0.539413680781759</v>
       </c>
     </row>
@@ -5413,11 +5908,11 @@
         <v>0</v>
       </c>
       <c r="M44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1552</v>
       </c>
       <c r="N44">
-        <f>(I44+J44*2+K44*3+L44*4)/M44</f>
+        <f t="shared" si="7"/>
         <v>0.54123711340206182</v>
       </c>
     </row>
@@ -5459,11 +5954,11 @@
         <v>0</v>
       </c>
       <c r="M45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1569</v>
       </c>
       <c r="N45">
-        <f>(I45+J45*2+K45*3+L45*4)/M45</f>
+        <f t="shared" si="7"/>
         <v>0.54110898661567874</v>
       </c>
     </row>
@@ -5505,11 +6000,11 @@
         <v>0</v>
       </c>
       <c r="M46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1578</v>
       </c>
       <c r="N46">
-        <f>(I46+J46*2+K46*3+L46*4)/M46</f>
+        <f t="shared" si="7"/>
         <v>0.54055766793409377</v>
       </c>
     </row>
@@ -5551,11 +6046,11 @@
         <v>0</v>
       </c>
       <c r="M47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1593</v>
       </c>
       <c r="N47">
-        <f>(I47+J47*2+K47*3+L47*4)/M47</f>
+        <f t="shared" si="7"/>
         <v>0.54300062774639046</v>
       </c>
     </row>
@@ -5597,11 +6092,11 @@
         <v>0</v>
       </c>
       <c r="M48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1611</v>
       </c>
       <c r="N48">
-        <f>(I48+J48*2+K48*3+L48*4)/M48</f>
+        <f t="shared" si="7"/>
         <v>0.54376163873370575</v>
       </c>
     </row>
@@ -5643,11 +6138,11 @@
         <v>0</v>
       </c>
       <c r="M49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1620</v>
       </c>
       <c r="N49">
-        <f>(I49+J49*2+K49*3+L49*4)/M49</f>
+        <f t="shared" si="7"/>
         <v>0.5419753086419753</v>
       </c>
     </row>
@@ -5689,11 +6184,11 @@
         <v>0</v>
       </c>
       <c r="M50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1630</v>
       </c>
       <c r="N50">
-        <f>(I50+J50*2+K50*3+L50*4)/M50</f>
+        <f t="shared" si="7"/>
         <v>0.54355828220858893</v>
       </c>
     </row>
@@ -5735,112 +6230,1162 @@
         <v>0</v>
       </c>
       <c r="M51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1640</v>
       </c>
       <c r="N51">
-        <f>(I51+J51*2+K51*3+L51*4)/M51</f>
+        <f t="shared" si="7"/>
         <v>0.54146341463414638</v>
       </c>
     </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52">
+        <v>0.33</v>
+      </c>
+      <c r="C52">
+        <v>0.33</v>
+      </c>
+      <c r="D52">
+        <v>0.33</v>
+      </c>
+      <c r="E52">
+        <v>100</v>
+      </c>
+      <c r="F52">
+        <v>20</v>
+      </c>
+      <c r="G52">
+        <v>0.64036188418999995</v>
+      </c>
+      <c r="H52">
+        <v>794</v>
+      </c>
+      <c r="I52">
+        <v>661</v>
+      </c>
+      <c r="J52">
+        <v>84</v>
+      </c>
+      <c r="K52">
+        <v>14</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <f t="shared" ref="M52:M76" si="8">SUM(H52:L52)</f>
+        <v>1553</v>
+      </c>
+      <c r="N52">
+        <f t="shared" ref="N52:N76" si="9">(I52+J52*2+K52*3+L52*4)/M52</f>
+        <v>0.56084996780424989</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53">
+        <v>0.33</v>
+      </c>
+      <c r="C53">
+        <v>0.33</v>
+      </c>
+      <c r="D53">
+        <v>0.33</v>
+      </c>
+      <c r="E53">
+        <v>100</v>
+      </c>
+      <c r="F53">
+        <v>40</v>
+      </c>
+      <c r="G53">
+        <v>0.63967587265299997</v>
+      </c>
+      <c r="H53">
+        <v>814</v>
+      </c>
+      <c r="I53">
+        <v>674</v>
+      </c>
+      <c r="J53">
+        <v>83</v>
+      </c>
+      <c r="K53">
+        <v>15</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="8"/>
+        <v>1586</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="9"/>
+        <v>0.55800756620428749</v>
+      </c>
+    </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54">
+        <v>0.33</v>
+      </c>
+      <c r="C54">
+        <v>0.33</v>
+      </c>
+      <c r="D54">
+        <v>0.33</v>
+      </c>
+      <c r="E54">
+        <v>100</v>
+      </c>
+      <c r="F54">
+        <v>60</v>
+      </c>
+      <c r="G54">
+        <v>0.63281929326999997</v>
+      </c>
+      <c r="H54">
+        <v>819</v>
+      </c>
+      <c r="I54">
+        <v>667</v>
+      </c>
+      <c r="J54">
+        <v>80</v>
+      </c>
+      <c r="K54">
+        <v>16</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
       <c r="M54">
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1582</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="9"/>
+        <v>0.55309734513274333</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55">
+        <v>0.33</v>
+      </c>
+      <c r="C55">
+        <v>0.33</v>
+      </c>
+      <c r="D55">
+        <v>0.33</v>
+      </c>
+      <c r="E55">
+        <v>100</v>
+      </c>
+      <c r="F55">
+        <v>80</v>
+      </c>
+      <c r="G55">
+        <v>0.63860196939000002</v>
+      </c>
+      <c r="H55">
+        <v>805</v>
+      </c>
+      <c r="I55">
+        <v>671</v>
+      </c>
+      <c r="J55">
+        <v>81</v>
+      </c>
+      <c r="K55">
+        <v>15</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
       <c r="M55">
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1572</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="9"/>
+        <v>0.55852417302798985</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56">
+        <v>0.33</v>
+      </c>
+      <c r="C56">
+        <v>0.33</v>
+      </c>
+      <c r="D56">
+        <v>0.33</v>
+      </c>
+      <c r="E56">
+        <v>100</v>
+      </c>
+      <c r="F56">
+        <v>100</v>
+      </c>
+      <c r="G56">
+        <v>0.63705571485800006</v>
+      </c>
+      <c r="H56">
+        <v>814</v>
+      </c>
+      <c r="I56">
+        <v>668</v>
+      </c>
+      <c r="J56">
+        <v>81</v>
+      </c>
+      <c r="K56">
+        <v>15</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
       <c r="M56">
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1578</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="9"/>
+        <v>0.55449936628643848</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57">
+        <v>0.33</v>
+      </c>
+      <c r="C57">
+        <v>0.33</v>
+      </c>
+      <c r="D57">
+        <v>0.33</v>
+      </c>
+      <c r="E57">
+        <v>100</v>
+      </c>
+      <c r="F57">
+        <v>120</v>
+      </c>
+      <c r="G57">
+        <v>0.63559681484599995</v>
+      </c>
+      <c r="H57">
+        <v>812</v>
+      </c>
+      <c r="I57">
+        <v>672</v>
+      </c>
+      <c r="J57">
+        <v>81</v>
+      </c>
+      <c r="K57">
+        <v>15</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
       <c r="M57">
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1580</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="9"/>
+        <v>0.5563291139240506</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58">
+        <v>0.33</v>
+      </c>
+      <c r="C58">
+        <v>0.33</v>
+      </c>
+      <c r="D58">
+        <v>0.33</v>
+      </c>
+      <c r="E58">
+        <v>100</v>
+      </c>
+      <c r="F58">
+        <v>140</v>
+      </c>
+      <c r="G58">
+        <v>0.63802119705399996</v>
+      </c>
+      <c r="H58">
+        <v>813</v>
+      </c>
+      <c r="I58">
+        <v>671</v>
+      </c>
+      <c r="J58">
+        <v>82</v>
+      </c>
+      <c r="K58">
+        <v>15</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
       <c r="M58">
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1581</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="9"/>
+        <v>0.55660974067046176</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59">
+        <v>0.33</v>
+      </c>
+      <c r="C59">
+        <v>0.33</v>
+      </c>
+      <c r="D59">
+        <v>0.33</v>
+      </c>
+      <c r="E59">
+        <v>100</v>
+      </c>
+      <c r="F59">
+        <v>160</v>
+      </c>
+      <c r="G59">
+        <v>0.63779668277099999</v>
+      </c>
+      <c r="H59">
+        <v>813</v>
+      </c>
+      <c r="I59">
+        <v>672</v>
+      </c>
+      <c r="J59">
+        <v>80</v>
+      </c>
+      <c r="K59">
+        <v>16</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
       <c r="M59">
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1581</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="9"/>
+        <v>0.55660974067046176</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60">
+        <v>0.33</v>
+      </c>
+      <c r="C60">
+        <v>0.33</v>
+      </c>
+      <c r="D60">
+        <v>0.33</v>
+      </c>
+      <c r="E60">
+        <v>100</v>
+      </c>
+      <c r="F60">
+        <v>180</v>
+      </c>
+      <c r="G60">
+        <v>0.636351915908</v>
+      </c>
+      <c r="H60">
+        <v>812</v>
+      </c>
+      <c r="I60">
+        <v>671</v>
+      </c>
+      <c r="J60">
+        <v>81</v>
+      </c>
+      <c r="K60">
+        <v>15</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
       <c r="M60">
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1579</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="9"/>
+        <v>0.55604813172894241</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61">
+        <v>0.33</v>
+      </c>
+      <c r="C61">
+        <v>0.33</v>
+      </c>
+      <c r="D61">
+        <v>0.33</v>
+      </c>
+      <c r="E61">
+        <v>100</v>
+      </c>
+      <c r="F61">
+        <v>200</v>
+      </c>
+      <c r="G61">
+        <v>0.63600506526099998</v>
+      </c>
+      <c r="H61">
+        <v>813</v>
+      </c>
+      <c r="I61">
+        <v>672</v>
+      </c>
+      <c r="J61">
+        <v>81</v>
+      </c>
+      <c r="K61">
+        <v>15</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
       <c r="M61">
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1581</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="9"/>
+        <v>0.55597722960151807</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62">
+        <v>0.33</v>
+      </c>
+      <c r="C62">
+        <v>0.33</v>
+      </c>
+      <c r="D62">
+        <v>0.33</v>
+      </c>
+      <c r="E62">
+        <v>10</v>
+      </c>
+      <c r="F62">
+        <v>100</v>
+      </c>
+      <c r="G62">
+        <v>0.64337080167399996</v>
+      </c>
+      <c r="H62">
+        <v>467</v>
+      </c>
+      <c r="I62">
+        <v>425</v>
+      </c>
+      <c r="J62">
+        <v>57</v>
+      </c>
+      <c r="K62">
+        <v>6</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
       <c r="M62">
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>955</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="9"/>
+        <v>0.58324607329842937</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63">
+        <v>0.33</v>
+      </c>
+      <c r="C63">
+        <v>0.33</v>
+      </c>
+      <c r="D63">
+        <v>0.33</v>
+      </c>
+      <c r="E63">
+        <v>20</v>
+      </c>
+      <c r="F63">
+        <v>100</v>
+      </c>
+      <c r="G63">
+        <v>0.647982783196</v>
+      </c>
+      <c r="H63">
+        <v>594</v>
+      </c>
+      <c r="I63">
+        <v>504</v>
+      </c>
+      <c r="J63">
+        <v>65</v>
+      </c>
+      <c r="K63">
+        <v>11</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
       <c r="M63">
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1174</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="9"/>
+        <v>0.56814310051107331</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64">
+        <v>0.33</v>
+      </c>
+      <c r="C64">
+        <v>0.33</v>
+      </c>
+      <c r="D64">
+        <v>0.33</v>
+      </c>
+      <c r="E64">
+        <v>30</v>
+      </c>
+      <c r="F64">
+        <v>100</v>
+      </c>
+      <c r="G64">
+        <v>0.64409474417199997</v>
+      </c>
+      <c r="H64">
+        <v>664</v>
+      </c>
+      <c r="I64">
+        <v>542</v>
+      </c>
+      <c r="J64">
+        <v>65</v>
+      </c>
+      <c r="K64">
+        <v>13</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
       <c r="M64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="13:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1284</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="9"/>
+        <v>0.55373831775700932</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65">
+        <v>0.33</v>
+      </c>
+      <c r="C65">
+        <v>0.33</v>
+      </c>
+      <c r="D65">
+        <v>0.33</v>
+      </c>
+      <c r="E65">
+        <v>40</v>
+      </c>
+      <c r="F65">
+        <v>100</v>
+      </c>
+      <c r="G65">
+        <v>0.64233188766399996</v>
+      </c>
+      <c r="H65">
+        <v>709</v>
+      </c>
+      <c r="I65">
+        <v>575</v>
+      </c>
+      <c r="J65">
+        <v>69</v>
+      </c>
+      <c r="K65">
+        <v>15</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
       <c r="M65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="13:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1368</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="9"/>
+        <v>0.55409356725146197</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>17</v>
+      </c>
+      <c r="B66">
+        <v>0.33</v>
+      </c>
+      <c r="C66">
+        <v>0.33</v>
+      </c>
+      <c r="D66">
+        <v>0.33</v>
+      </c>
+      <c r="E66">
+        <v>50</v>
+      </c>
+      <c r="F66">
+        <v>100</v>
+      </c>
+      <c r="G66">
+        <v>0.63864301690299996</v>
+      </c>
+      <c r="H66">
+        <v>748</v>
+      </c>
+      <c r="I66">
+        <v>593</v>
+      </c>
+      <c r="J66">
+        <v>79</v>
+      </c>
+      <c r="K66">
+        <v>13</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
       <c r="M66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="13:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1433</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="9"/>
+        <v>0.55129099790648983</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67">
+        <v>0.33</v>
+      </c>
+      <c r="C67">
+        <v>0.33</v>
+      </c>
+      <c r="D67">
+        <v>0.33</v>
+      </c>
+      <c r="E67">
+        <v>60</v>
+      </c>
+      <c r="F67">
+        <v>100</v>
+      </c>
+      <c r="G67">
+        <v>0.63645889307400005</v>
+      </c>
+      <c r="H67">
+        <v>777</v>
+      </c>
+      <c r="I67">
+        <v>634</v>
+      </c>
+      <c r="J67">
+        <v>77</v>
+      </c>
+      <c r="K67">
+        <v>14</v>
+      </c>
+      <c r="L67">
+        <v>0</v>
+      </c>
       <c r="M67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="13:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1502</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="9"/>
+        <v>0.55259653794940078</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>17</v>
+      </c>
+      <c r="B68">
+        <v>0.33</v>
+      </c>
+      <c r="C68">
+        <v>0.33</v>
+      </c>
+      <c r="D68">
+        <v>0.33</v>
+      </c>
+      <c r="E68">
+        <v>70</v>
+      </c>
+      <c r="F68">
+        <v>100</v>
+      </c>
+      <c r="G68">
+        <v>0.63807034950300001</v>
+      </c>
+      <c r="H68">
+        <v>786</v>
+      </c>
+      <c r="I68">
+        <v>655</v>
+      </c>
+      <c r="J68">
+        <v>79</v>
+      </c>
+      <c r="K68">
+        <v>14</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
       <c r="M68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="13:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1534</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="9"/>
+        <v>0.55736636245110827</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>17</v>
+      </c>
+      <c r="B69">
+        <v>0.33</v>
+      </c>
+      <c r="C69">
+        <v>0.33</v>
+      </c>
+      <c r="D69">
+        <v>0.33</v>
+      </c>
+      <c r="E69">
+        <v>80</v>
+      </c>
+      <c r="F69">
+        <v>100</v>
+      </c>
+      <c r="G69">
+        <v>0.64224702654499999</v>
+      </c>
+      <c r="H69">
+        <v>797</v>
+      </c>
+      <c r="I69">
+        <v>657</v>
+      </c>
+      <c r="J69">
+        <v>82</v>
+      </c>
+      <c r="K69">
+        <v>15</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
       <c r="M69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="13:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1551</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="9"/>
+        <v>0.55834945196647323</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70">
+        <v>0.33</v>
+      </c>
+      <c r="C70">
+        <v>0.33</v>
+      </c>
+      <c r="D70">
+        <v>0.33</v>
+      </c>
+      <c r="E70">
+        <v>90</v>
+      </c>
+      <c r="F70">
+        <v>100</v>
+      </c>
+      <c r="G70">
+        <v>0.64171608867700003</v>
+      </c>
+      <c r="H70">
+        <v>807</v>
+      </c>
+      <c r="I70">
+        <v>664</v>
+      </c>
+      <c r="J70">
+        <v>82</v>
+      </c>
+      <c r="K70">
+        <v>15</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
       <c r="M70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="13:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1568</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="9"/>
+        <v>0.55676020408163263</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71">
+        <v>0.33</v>
+      </c>
+      <c r="C71">
+        <v>0.33</v>
+      </c>
+      <c r="D71">
+        <v>0.33</v>
+      </c>
+      <c r="E71">
+        <v>100</v>
+      </c>
+      <c r="F71">
+        <v>100</v>
+      </c>
+      <c r="G71">
+        <v>0.63705571485800006</v>
+      </c>
+      <c r="H71">
+        <v>814</v>
+      </c>
+      <c r="I71">
+        <v>668</v>
+      </c>
+      <c r="J71">
+        <v>81</v>
+      </c>
+      <c r="K71">
+        <v>15</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
       <c r="M71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="13:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1578</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="9"/>
+        <v>0.55449936628643848</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>17</v>
+      </c>
+      <c r="B72">
+        <v>0.33</v>
+      </c>
+      <c r="C72">
+        <v>0.33</v>
+      </c>
+      <c r="D72">
+        <v>0.33</v>
+      </c>
+      <c r="E72">
+        <v>110</v>
+      </c>
+      <c r="F72">
+        <v>100</v>
+      </c>
+      <c r="G72">
+        <v>0.63750908140100004</v>
+      </c>
+      <c r="H72">
+        <v>821</v>
+      </c>
+      <c r="I72">
+        <v>673</v>
+      </c>
+      <c r="J72">
+        <v>83</v>
+      </c>
+      <c r="K72">
+        <v>16</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
       <c r="M72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="13:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1593</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="9"/>
+        <v>0.5568110483364721</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>17</v>
+      </c>
+      <c r="B73">
+        <v>0.33</v>
+      </c>
+      <c r="C73">
+        <v>0.33</v>
+      </c>
+      <c r="D73">
+        <v>0.33</v>
+      </c>
+      <c r="E73">
+        <v>120</v>
+      </c>
+      <c r="F73">
+        <v>100</v>
+      </c>
+      <c r="G73">
+        <v>0.63686245617799997</v>
+      </c>
+      <c r="H73">
+        <v>828</v>
+      </c>
+      <c r="I73">
+        <v>683</v>
+      </c>
+      <c r="J73">
+        <v>85</v>
+      </c>
+      <c r="K73">
+        <v>15</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
       <c r="M73">
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1611</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="9"/>
+        <v>0.55741775294847917</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>17</v>
+      </c>
+      <c r="B74">
+        <v>0.33</v>
+      </c>
+      <c r="C74">
+        <v>0.33</v>
+      </c>
+      <c r="D74">
+        <v>0.33</v>
+      </c>
+      <c r="E74">
+        <v>130</v>
+      </c>
+      <c r="F74">
+        <v>100</v>
+      </c>
+      <c r="G74">
+        <v>0.63204954909</v>
+      </c>
+      <c r="H74">
+        <v>831</v>
+      </c>
+      <c r="I74">
+        <v>690</v>
+      </c>
+      <c r="J74">
+        <v>85</v>
+      </c>
+      <c r="K74">
+        <v>14</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <f t="shared" si="8"/>
+        <v>1620</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="9"/>
+        <v>0.55679012345679013</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>17</v>
+      </c>
+      <c r="B75">
+        <v>0.33</v>
+      </c>
+      <c r="C75">
+        <v>0.33</v>
+      </c>
+      <c r="D75">
+        <v>0.33</v>
+      </c>
+      <c r="E75">
+        <v>140</v>
+      </c>
+      <c r="F75">
+        <v>100</v>
+      </c>
+      <c r="G75">
+        <v>0.63469454315600005</v>
+      </c>
+      <c r="H75">
+        <v>836</v>
+      </c>
+      <c r="I75">
+        <v>694</v>
+      </c>
+      <c r="J75">
+        <v>87</v>
+      </c>
+      <c r="K75">
+        <v>13</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <f t="shared" si="8"/>
+        <v>1630</v>
+      </c>
+      <c r="N75">
+        <f t="shared" si="9"/>
+        <v>0.55644171779141105</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>17</v>
+      </c>
+      <c r="B76">
+        <v>0.33</v>
+      </c>
+      <c r="C76">
+        <v>0.33</v>
+      </c>
+      <c r="D76">
+        <v>0.33</v>
+      </c>
+      <c r="E76">
+        <v>150</v>
+      </c>
+      <c r="F76">
+        <v>100</v>
+      </c>
+      <c r="G76">
+        <v>0.63416869797700004</v>
+      </c>
+      <c r="H76">
+        <v>836</v>
+      </c>
+      <c r="I76">
+        <v>706</v>
+      </c>
+      <c r="J76">
+        <v>85</v>
+      </c>
+      <c r="K76">
+        <v>13</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <f t="shared" si="8"/>
+        <v>1640</v>
+      </c>
+      <c r="N76">
+        <f t="shared" si="9"/>
+        <v>0.55792682926829273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done editing the report
</commit_message>
<xml_diff>
--- a/Results/results2.xlsx
+++ b/Results/results2.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="22">
   <si>
     <t>userW</t>
   </si>
@@ -72,7 +73,19 @@
     <t>err</t>
   </si>
   <si>
-    <t>all</t>
+    <t>original</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Original Alg</t>
+  </si>
+  <si>
+    <t>New Alg</t>
+  </si>
+  <si>
+    <t>Rounded MSE</t>
   </si>
 </sst>
 </file>
@@ -1116,11 +1129,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="382829224"/>
-        <c:axId val="382833536"/>
+        <c:axId val="371814288"/>
+        <c:axId val="371813896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="382829224"/>
+        <c:axId val="371814288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1209,12 +1222,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382833536"/>
+        <c:crossAx val="371813896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="382833536"/>
+        <c:axId val="371813896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1306,7 +1319,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382829224"/>
+        <c:crossAx val="371814288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1782,11 +1795,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="469657576"/>
-        <c:axId val="469662280"/>
+        <c:axId val="371808800"/>
+        <c:axId val="371803704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="469657576"/>
+        <c:axId val="371808800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1880,12 +1893,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="469662280"/>
+        <c:crossAx val="371803704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="469662280"/>
+        <c:axId val="371803704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.75000000000000011"/>
@@ -1979,7 +1992,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="469657576"/>
+        <c:crossAx val="371808800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2450,11 +2463,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="382842552"/>
-        <c:axId val="382841376"/>
+        <c:axId val="371809584"/>
+        <c:axId val="374642304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="382842552"/>
+        <c:axId val="371809584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2548,12 +2561,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382841376"/>
+        <c:crossAx val="374642304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="382841376"/>
+        <c:axId val="374642304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.65500000000000014"/>
@@ -2647,7 +2660,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382842552"/>
+        <c:crossAx val="371809584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3210,11 +3223,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="379131736"/>
-        <c:axId val="379133304"/>
+        <c:axId val="374637992"/>
+        <c:axId val="374640344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="379131736"/>
+        <c:axId val="374637992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3303,12 +3316,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379133304"/>
+        <c:crossAx val="374640344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="379133304"/>
+        <c:axId val="374640344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3400,7 +3413,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379131736"/>
+        <c:crossAx val="374637992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3513,16 +3526,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>323849</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>542924</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3543,16 +3556,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3869,8 +3882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N71" sqref="N71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7379,4 +7392,63 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>0.61829999999999996</v>
+      </c>
+      <c r="C2">
+        <v>0.69140000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>0.6371</v>
+      </c>
+      <c r="C3">
+        <v>0.71419999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>0.62109999999999999</v>
+      </c>
+      <c r="C4">
+        <v>0.68689999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>